<commit_message>
Cookie, Ticket, Point 모델 Generate
</commit_message>
<xml_diff>
--- a/Data/Excel/Model/Player.xlsx
+++ b/Data/Excel/Model/Player.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAA5AD5-FFFC-48B7-92D4-B62CF5FC7D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F719104-265A-4A62-95E3-A7BA21BDF62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -170,6 +170,30 @@
   </si>
   <si>
     <t>LIST:KingdomObjPacket</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CookieList</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PointList</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TicketList</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIST:CookiePacket</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIST:PointPacket</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIST:TicketPacket</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1104,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC6768-C9E8-4795-B55A-C1C942DE1B76}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1344,6 +1368,39 @@
         <v>33</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>